<commit_message>
update biogas plant ID
</commit_message>
<xml_diff>
--- a/dig_prop_data/digestate_comp.xlsx
+++ b/dig_prop_data/digestate_comp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{B99391DA-0905-48EC-93E3-B7564715C564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E4DDEEF-50F1-407B-87FB-DB013500F34F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{B99391DA-0905-48EC-93E3-B7564715C564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F3D7C1-6E35-4ADD-8873-144D32FF1C38}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3045" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Johanna - compact" sheetId="16" r:id="rId1"/>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -197,33 +197,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +501,7 @@
     <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -549,7 +522,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -570,7 +543,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
@@ -591,7 +564,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -612,7 +585,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
@@ -633,7 +606,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
@@ -641,7 +614,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>7.89</v>
@@ -654,7 +627,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -662,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>8.24</v>
@@ -675,7 +648,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -683,21 +656,20 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>6</v>
-      </c>
-      <c r="D8" s="13">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="3">
         <v>8.6747595377452864</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="3">
         <v>2.9914529914529915</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -705,65 +677,62 @@
         <v>6</v>
       </c>
       <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11.22907780019418</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.4257425742574257</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
         <v>7</v>
       </c>
-      <c r="D9" s="12">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="E9" s="13">
-        <v>11.22907780019418</v>
-      </c>
-      <c r="F9" s="13">
-        <v>2.4257425742574257</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6.1527822682041879</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3.6417322834645671</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="12">
-        <v>8.4</v>
-      </c>
-      <c r="E10" s="13">
-        <v>6.1527822682041879</v>
-      </c>
-      <c r="F10" s="13">
-        <v>3.6417322834645671</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1">
-        <v>9</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="D11" s="1">
         <v>7.94</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="3">
         <v>6.024897680763984</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="3">
         <v>2.0236920039486672</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>9</v>
       </c>
@@ -771,307 +740,290 @@
         <v>6</v>
       </c>
       <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8.08</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6.946519599226578</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3.1663516068052928</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="12">
-        <v>8.08</v>
-      </c>
-      <c r="E12" s="13">
-        <v>6.946519599226578</v>
-      </c>
-      <c r="F12" s="13">
-        <v>3.1663516068052928</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
+        <v>7.82</v>
+      </c>
+      <c r="E13" s="3">
+        <v>6.5367375637194591</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3.8613861386138613</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
         <v>11</v>
       </c>
-      <c r="D13" s="12">
-        <v>7.82</v>
-      </c>
-      <c r="E13" s="13">
-        <v>6.5367375637194591</v>
-      </c>
-      <c r="F13" s="13">
-        <v>3.8613861386138613</v>
-      </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
+        <v>8.06</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5.6996896835616724</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.9705882352941178</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
         <v>12</v>
       </c>
-      <c r="D14" s="12">
-        <v>8.06</v>
-      </c>
-      <c r="E14" s="13">
-        <v>5.6996896835616724</v>
-      </c>
-      <c r="F14" s="13">
-        <v>3.9705882352941178</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="E15" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.3949169110459434</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1">
         <v>13</v>
       </c>
-      <c r="D15" s="12">
-        <v>7.89</v>
-      </c>
-      <c r="E15" s="12">
-        <v>8.75</v>
-      </c>
-      <c r="F15" s="13">
-        <v>2.3949169110459434</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E16" s="3">
+        <v>4.3661752158316283</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3.6654135338345863</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
         <v>14</v>
       </c>
-      <c r="D16" s="12">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E16" s="13">
-        <v>4.3661752158316283</v>
-      </c>
-      <c r="F16" s="13">
-        <v>3.6654135338345863</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
+        <v>7.92</v>
+      </c>
+      <c r="E17" s="3">
+        <v>6.7437576087926558</v>
+      </c>
+      <c r="F17" s="3">
+        <v>4.1794423201789197</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="E18" s="3">
+        <v>4.3635266396361558</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3.1278557114228454</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
         <v>15</v>
       </c>
-      <c r="D17" s="12">
-        <v>7.92</v>
-      </c>
-      <c r="E17" s="13">
-        <v>6.7437576087926558</v>
-      </c>
-      <c r="F17" s="13">
-        <v>4.1794423201789197</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="D19" s="1">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7.8532600789520917</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2.3488847700521314</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1">
+        <v>8.02</v>
+      </c>
+      <c r="E20" s="3">
+        <v>7.1349871478067577</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2.8971552214786178</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7.93</v>
+      </c>
+      <c r="E21" s="3">
+        <v>6.6897912981169867</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2.4434118792057733</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1">
         <v>16</v>
       </c>
-      <c r="D18" s="12">
-        <v>7.58</v>
-      </c>
-      <c r="E18" s="13">
-        <v>4.3635266396361558</v>
-      </c>
-      <c r="F18" s="13">
-        <v>3.1278557114228454</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="16"/>
-    </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="D22" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="E22" s="3">
+        <v>7.2383016080668607</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2.4941130221705441</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
         <v>17</v>
       </c>
-      <c r="D19" s="12">
-        <v>8.2899999999999991</v>
-      </c>
-      <c r="E19" s="13">
-        <v>7.8532600789520917</v>
-      </c>
-      <c r="F19" s="13">
-        <v>2.3488847700521314</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="D23" s="1">
+        <v>7.98</v>
+      </c>
+      <c r="E23" s="3">
+        <v>5.388140612173558</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2.933717344029664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1">
         <v>18</v>
       </c>
-      <c r="D20" s="12">
-        <v>8.02</v>
-      </c>
-      <c r="E20" s="13">
-        <v>7.1349871478067577</v>
-      </c>
-      <c r="F20" s="13">
-        <v>2.8971552214786178</v>
-      </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="D24" s="1">
+        <v>7.93</v>
+      </c>
+      <c r="E24" s="3">
+        <v>8.6591343775030616</v>
+      </c>
+      <c r="F24" s="3">
+        <v>3.0371485943775101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1">
         <v>19</v>
       </c>
-      <c r="D21" s="12">
-        <v>7.93</v>
-      </c>
-      <c r="E21" s="13">
-        <v>6.6897912981169867</v>
-      </c>
-      <c r="F21" s="13">
-        <v>2.4434118792057733</v>
-      </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="14"/>
-    </row>
-    <row r="22" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1">
-        <v>20</v>
-      </c>
-      <c r="D22" s="12">
-        <v>7.99</v>
-      </c>
-      <c r="E22" s="13">
-        <v>7.2383016080668607</v>
-      </c>
-      <c r="F22" s="13">
-        <v>2.4941130221705441</v>
-      </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="18"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1">
-        <v>21</v>
-      </c>
-      <c r="D23" s="12">
-        <v>7.98</v>
-      </c>
-      <c r="E23" s="13">
-        <v>5.388140612173558</v>
-      </c>
-      <c r="F23" s="13">
-        <v>2.933717344029664</v>
-      </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1">
-        <v>22</v>
-      </c>
-      <c r="D24" s="12">
-        <v>7.93</v>
-      </c>
-      <c r="E24" s="13">
-        <v>8.6591343775030616</v>
-      </c>
-      <c r="F24" s="13">
-        <v>3.0371485943775101</v>
-      </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1">
-        <v>23</v>
-      </c>
-      <c r="D25" s="12">
+      <c r="D25" s="1">
         <v>7.96</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="3">
         <v>6.1322937109949667</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="3">
         <v>2.3363619277489809</v>
       </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>10</v>
       </c>
@@ -1079,21 +1031,20 @@
         <v>6</v>
       </c>
       <c r="C26" s="1">
-        <v>24</v>
-      </c>
-      <c r="D26" s="12">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1">
         <v>7.98</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="1">
         <v>8.0299999999999994</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="1">
         <v>2.65</v>
       </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="18"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>10</v>
       </c>
@@ -1101,21 +1052,20 @@
         <v>6</v>
       </c>
       <c r="C27" s="1">
-        <v>25</v>
-      </c>
-      <c r="D27" s="12">
+        <v>20</v>
+      </c>
+      <c r="D27" s="1">
         <v>7.98</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="1">
         <v>7.27</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="1">
         <v>2.5499999999999998</v>
       </c>
-      <c r="G27" s="13"/>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>10</v>
       </c>
@@ -1123,21 +1073,20 @@
         <v>6</v>
       </c>
       <c r="C28" s="1">
-        <v>26</v>
-      </c>
-      <c r="D28" s="12">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1">
         <v>7.86</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="1">
         <v>9.15</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="1">
         <v>2.4</v>
       </c>
-      <c r="G28" s="13"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" s="4" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>10</v>
       </c>
@@ -1145,21 +1094,20 @@
         <v>6</v>
       </c>
       <c r="C29" s="1">
-        <v>27</v>
-      </c>
-      <c r="D29" s="12">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
         <v>8.49</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="1">
         <v>5.57</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="1">
         <v>2.5499999999999998</v>
       </c>
-      <c r="G29" s="13"/>
-      <c r="H29" s="19"/>
-    </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>10</v>
       </c>
@@ -1167,21 +1115,20 @@
         <v>6</v>
       </c>
       <c r="C30" s="1">
-        <v>28</v>
-      </c>
-      <c r="D30" s="12">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1">
         <v>8.0299999999999994</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="1">
         <v>9.07</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="1">
         <v>2.38</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="20"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>10</v>
       </c>
@@ -1189,21 +1136,20 @@
         <v>6</v>
       </c>
       <c r="C31" s="1">
-        <v>29</v>
-      </c>
-      <c r="D31" s="13">
+        <v>22</v>
+      </c>
+      <c r="D31" s="3">
         <v>8</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="1">
         <v>8.9700000000000006</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="1">
         <v>3.63</v>
       </c>
-      <c r="G31" s="13"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>10</v>
       </c>
@@ -1211,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="1">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D32" s="1">
         <v>8.2100000000000009</v>
@@ -1232,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="1">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D33" s="1">
         <v>7.81</v>

</xml_diff>

<commit_message>
fixing error in digestate_comp
</commit_message>
<xml_diff>
--- a/dig_prop_data/digestate_comp.xlsx
+++ b/dig_prop_data/digestate_comp.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{B99391DA-0905-48EC-93E3-B7564715C564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F3D7C1-6E35-4ADD-8873-144D32FF1C38}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{B99391DA-0905-48EC-93E3-B7564715C564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{407241BA-6005-4E62-B4A3-9834E29B5BF8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -197,6 +197,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +504,7 @@
     <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -522,7 +525,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -543,7 +546,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
@@ -564,7 +567,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -585,7 +588,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
@@ -606,7 +609,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
@@ -623,11 +626,11 @@
         <v>5.4831450660606462</v>
       </c>
       <c r="F6" s="3">
-        <v>1.0620000000000001</v>
+        <v>2.88</v>
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -647,8 +650,9 @@
         <v>4.375</v>
       </c>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -669,7 +673,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -690,7 +694,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
@@ -711,7 +715,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
@@ -732,7 +736,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>9</v>
       </c>
@@ -753,7 +757,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
@@ -774,7 +778,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
@@ -795,7 +799,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
@@ -816,7 +820,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>9</v>
       </c>

</xml_diff>